<commit_message>
Gesamtdoku Dokumente und Udos Kritik
</commit_message>
<xml_diff>
--- a/Gesamtdoku/Verbesserungsmöglichkeiten/Übersicht Verbesserungsmöglichkeiten.xlsx
+++ b/Gesamtdoku/Verbesserungsmöglichkeiten/Übersicht Verbesserungsmöglichkeiten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\Methodisches Konstruieren\Übungen\git repo\MKon\Gesamtdoku\Verbesserungsmöglichkeiten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062E48AC-714D-4C0A-8113-B9EE268930C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33053AAC-095E-4823-A063-5C30331074C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1FF97F9F-C11D-4C51-B887-11B35ED066E3}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1FF97F9F-C11D-4C51-B887-11B35ED066E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
   <dimension ref="B3:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>